<commit_message>
fixed gumbel issue, trying to fix log1mexp?
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Github\fmax\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9DA87A-E885-4675-897B-192B5BBC4A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F438CF4-29EF-4EBF-9E37-21999B1E3FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="2475" windowWidth="35160" windowHeight="15435" activeTab="1" xr2:uid="{B3B789DA-C08B-4A7D-9B2B-1AC8450A05A4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B3B789DA-C08B-4A7D-9B2B-1AC8450A05A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Gaussian_forecasts" sheetId="1" r:id="rId1"/>
     <sheet name="Gumbel_forecasts" sheetId="2" r:id="rId2"/>
+    <sheet name="Gaussian Olympic" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>event</t>
   </si>
@@ -59,6 +60,54 @@
   </si>
   <si>
     <t>Marathon</t>
+  </si>
+  <si>
+    <t>MSEs:</t>
+  </si>
+  <si>
+    <t>Average logp on hold out:</t>
+  </si>
+  <si>
+    <t>Training was first 20 data points</t>
+  </si>
+  <si>
+    <t>100 metres, Men</t>
+  </si>
+  <si>
+    <t>400 metres, Men</t>
+  </si>
+  <si>
+    <t>800 metres, Men</t>
+  </si>
+  <si>
+    <t>110 metres Hurdles, Men : 0.06377592219848145</t>
+  </si>
+  <si>
+    <t>200 metres, Men</t>
+  </si>
+  <si>
+    <t>400 metres Hurdles, Men</t>
+  </si>
+  <si>
+    <t>1,500 metres, Men</t>
+  </si>
+  <si>
+    <t>5,000 metres, Men</t>
+  </si>
+  <si>
+    <t>4 x 100 metres Relay, Men</t>
+  </si>
+  <si>
+    <t>4 x 400 metres Relay, Men</t>
+  </si>
+  <si>
+    <t>3,000 metres Steeplechase, Men</t>
+  </si>
+  <si>
+    <t>100 metres, Women</t>
+  </si>
+  <si>
+    <t>110 metres Hurdles, Men</t>
   </si>
 </sst>
 </file>
@@ -502,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E76B38-D840-4EF1-A8E6-143FCE3D9ED9}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -545,4 +594,230 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B3E1B3-6BB2-4E74-BF06-292686E318D0}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>6.7224457779073996E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0.16619999999999599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1.10737252809609</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>6.3775922198481397E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>0.16170381418090601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>0.176333333333339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>45.279674999999699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>0.156799999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>9.1875000000011905E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1.6576333333333599</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>-7.1487083884933096</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>-10.7229850624663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>-12.0064475038676</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>-9.7046885047827995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>-6.7996248520653699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <v>-3.1620820157848599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>-10.1513154439119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>-15.953386773586899</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>-5.5655457085016602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>-8.6598274347477897</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>-13.426897982511599</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>-1.7103210301987599</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Big update.... working gumbel
</commit_message>
<xml_diff>
--- a/notebooks/results.xlsx
+++ b/notebooks/results.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Github\fmax\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F438CF4-29EF-4EBF-9E37-21999B1E3FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D32D94-A9A3-49A7-9742-0F53F1F702AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B3B789DA-C08B-4A7D-9B2B-1AC8450A05A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3B789DA-C08B-4A7D-9B2B-1AC8450A05A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Gaussian_forecasts" sheetId="1" r:id="rId1"/>
+    <sheet name="Forecast Results" sheetId="1" r:id="rId1"/>
     <sheet name="Gumbel_forecasts" sheetId="2" r:id="rId2"/>
     <sheet name="Gaussian Olympic" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>event</t>
   </si>
@@ -108,14 +108,31 @@
   </si>
   <si>
     <t>110 metres Hurdles, Men</t>
+  </si>
+  <si>
+    <t>Gaussian</t>
+  </si>
+  <si>
+    <t>Gumbell</t>
+  </si>
+  <si>
+    <t>10000m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,10 +148,48 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -143,8 +198,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,87 +520,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1FEAA8-8DA0-4A9F-AFF6-BAE82D1955C6}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="3" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="1">
         <v>-2.5125023009428098</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>0.113798530991551</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="6">
+        <v>-2.3133238337438198</v>
+      </c>
+      <c r="E3">
+        <v>0.180922286554279</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.30973333333333802</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>-14.449838462740599</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>2.5842323019458799</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="1">
+        <v>-34.975430175754497</v>
+      </c>
+      <c r="E4">
+        <v>2.4401370104325601</v>
+      </c>
+      <c r="F4" s="1">
         <v>1.9230733333333501</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="1">
         <v>-66.457770786825094</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>65.493526666666298</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="1">
+        <v>-253.719062462712</v>
+      </c>
+      <c r="E5">
+        <v>56.131603835474898</v>
+      </c>
+      <c r="F5" s="1">
         <v>43.370706666666699</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B6" s="1">
         <v>-72.281028989982602</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>5341.1333333333296</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="1">
+        <v>-34.724935845015402</v>
+      </c>
+      <c r="E6">
+        <v>1357.3136428937501</v>
+      </c>
+      <c r="F6" s="1">
         <v>3500.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>-307.73366317753499</v>
+      </c>
+      <c r="C7" s="5">
+        <v>607.34181333333697</v>
+      </c>
+      <c r="D7">
+        <v>-20798.324907738301</v>
+      </c>
+      <c r="E7" s="5">
+        <v>524.43402557712204</v>
+      </c>
+      <c r="F7">
+        <v>496.97074666666703</v>
       </c>
     </row>
   </sheetData>
@@ -556,6 +679,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -601,8 +729,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>